<commit_message>
small tweaks with the names
small tweaks with the names
</commit_message>
<xml_diff>
--- a/assets/Asset template.xlsx
+++ b/assets/Asset template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krameshbabu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\My_Intern\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>S.No.</t>
   </si>
@@ -228,6 +228,81 @@
   </si>
   <si>
     <t>Unassigned</t>
+  </si>
+  <si>
+    <t>sno</t>
+  </si>
+  <si>
+    <t>SeatNo</t>
+  </si>
+  <si>
+    <t>EmpID</t>
+  </si>
+  <si>
+    <t>EmpNm</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>atn</t>
+  </si>
+  <si>
+    <t>Asstyp</t>
+  </si>
+  <si>
+    <t>HostNm</t>
+  </si>
+  <si>
+    <t>Loc</t>
+  </si>
+  <si>
+    <t>SrlNo</t>
+  </si>
+  <si>
+    <t>AssDev</t>
+  </si>
+  <si>
+    <t>ADSNo</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>Mem</t>
+  </si>
+  <si>
+    <t>Proc</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PurchOn</t>
+  </si>
+  <si>
+    <t>Inv</t>
+  </si>
+  <si>
+    <t>Vend</t>
+  </si>
+  <si>
+    <t>Wrty</t>
+  </si>
+  <si>
+    <t>DoI</t>
+  </si>
+  <si>
+    <t>Cno</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Rmks</t>
   </si>
 </sst>
 </file>
@@ -643,7 +718,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,6 +1010,89 @@
         <v>59</v>
       </c>
     </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>82</v>
+      </c>
+      <c r="R16" t="s">
+        <v>83</v>
+      </c>
+      <c r="S16" t="s">
+        <v>84</v>
+      </c>
+      <c r="T16" t="s">
+        <v>85</v>
+      </c>
+      <c r="U16" t="s">
+        <v>86</v>
+      </c>
+      <c r="V16" t="s">
+        <v>87</v>
+      </c>
+      <c r="W16" t="s">
+        <v>88</v>
+      </c>
+      <c r="X16" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
     </row>

</xml_diff>